<commit_message>
Adding misc feature analysis
Added user features
</commit_message>
<xml_diff>
--- a/resultsDump/sayantan/featureTTestResults.xlsx
+++ b/resultsDump/sayantan/featureTTestResults.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>rhyme</t>
   </si>
@@ -59,6 +59,18 @@
   </si>
   <si>
     <t>NaN</t>
+  </si>
+  <si>
+    <t>user_favcount</t>
+  </si>
+  <si>
+    <t>user_followercount</t>
+  </si>
+  <si>
+    <t>user_friendsCount</t>
+  </si>
+  <si>
+    <t>user_statusCount</t>
   </si>
 </sst>
 </file>
@@ -416,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,6 +590,146 @@
         <v>0.15679999999999999</v>
       </c>
     </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1.5E-3</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0.30549999999999999</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>4.8429000000000001E-4</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0.90359999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0.1731</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0.1958</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0.20760000000000001</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0.26</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0.3649</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0.15820000000000001</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0.58209999999999995</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0.92230000000000001</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>9.1899999999999996E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.46E-2</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0.1424</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>2.5700000000000001E-2</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Renaming simplesentiment to simpleconnotation
Also adding connotation file
</commit_message>
<xml_diff>
--- a/resultsDump/sayantan/featureTTestResults.xlsx
+++ b/resultsDump/sayantan/featureTTestResults.xlsx
@@ -73,9 +73,6 @@
     <t>user_statusCount</t>
   </si>
   <si>
-    <t>simplesentiment</t>
-  </si>
-  <si>
     <t>f6 pass</t>
   </si>
   <si>
@@ -86,6 +83,9 @@
   </si>
   <si>
     <t>f7 p value</t>
+  </si>
+  <si>
+    <t>simpleconnotation</t>
   </si>
 </sst>
 </file>
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,16 +483,16 @@
         <v>12</v>
       </c>
       <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
         <v>20</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>22</v>
-      </c>
-      <c r="O1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -759,7 +759,7 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B10" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Add sentiment analysis based on AFINN
</commit_message>
<xml_diff>
--- a/resultsDump/sayantan/featureTTestResults.xlsx
+++ b/resultsDump/sayantan/featureTTestResults.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>rhyme</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>rhyme (hashtag separated)</t>
+  </si>
+  <si>
+    <t>afinn</t>
   </si>
 </sst>
 </file>
@@ -446,15 +449,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:AE12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>4</v>
       </c>
@@ -498,7 +501,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -533,7 +536,7 @@
         <v>2.2000000000000001E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -568,7 +571,7 @@
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -597,7 +600,7 @@
         <v>5.3720000000000004E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -620,7 +623,7 @@
         <v>0.15679999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -655,7 +658,7 @@
         <v>0.90359999999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -690,7 +693,7 @@
         <v>0.3649</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -725,7 +728,7 @@
         <v>9.1899999999999996E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -760,7 +763,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -807,7 +810,7 @@
         <v>0.57189999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -834,6 +837,101 @@
       </c>
       <c r="I11" s="1">
         <v>4.7873000000000001E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>9.339599999999999E-44</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1.0468E-48</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1.5352E-76</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1">
+        <v>3.8665000000000002E-13</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0.37559999999999999</v>
+      </c>
+      <c r="N12" s="2">
+        <v>1</v>
+      </c>
+      <c r="O12" s="1">
+        <v>1.0890999999999999E-104</v>
+      </c>
+      <c r="P12" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>6.7100000000000001E-60</v>
+      </c>
+      <c r="R12" s="2">
+        <v>1</v>
+      </c>
+      <c r="S12" s="1">
+        <v>2.8983000000000002E-28</v>
+      </c>
+      <c r="T12" s="2">
+        <v>1</v>
+      </c>
+      <c r="U12" s="1">
+        <v>3.3134999999999998E-38</v>
+      </c>
+      <c r="V12" s="2">
+        <v>1</v>
+      </c>
+      <c r="W12" s="1">
+        <v>2.9907999999999999E-5</v>
+      </c>
+      <c r="X12" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>4.4576000000000002E-98</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>7.7499999999999999E-2</v>
+      </c>
+      <c r="AB12" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>3.9390999999999997E-4</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>0.2437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding corrected AFINN features
</commit_message>
<xml_diff>
--- a/resultsDump/sayantan/featureTTestResults.xlsx
+++ b/resultsDump/sayantan/featureTTestResults.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>rhyme</t>
   </si>
@@ -451,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,71 +849,71 @@
       <c r="C12" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="2">
-        <v>1</v>
+      <c r="D12">
+        <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>9.339599999999999E-44</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1</v>
+        <v>0.28989999999999999</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
       </c>
       <c r="G12" s="1">
-        <v>1.0468E-48</v>
-      </c>
-      <c r="H12" s="2">
-        <v>1</v>
+        <v>0.8</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
       </c>
       <c r="I12" s="1">
-        <v>1.5352E-76</v>
-      </c>
-      <c r="J12" s="2">
-        <v>1</v>
+        <v>0.4627</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
       </c>
       <c r="K12" s="1">
-        <v>3.8665000000000002E-13</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>0.37559999999999999</v>
-      </c>
-      <c r="N12" s="2">
-        <v>1</v>
+        <v>0.6179</v>
+      </c>
+      <c r="L12" t="s">
+        <v>14</v>
+      </c>
+      <c r="M12" t="s">
+        <v>14</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
       </c>
       <c r="O12" s="1">
-        <v>1.0890999999999999E-104</v>
-      </c>
-      <c r="P12" s="2">
-        <v>1</v>
+        <v>0.41060000000000002</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
       </c>
       <c r="Q12" s="1">
-        <v>6.7100000000000001E-60</v>
-      </c>
-      <c r="R12" s="2">
-        <v>1</v>
+        <v>0.53910000000000002</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
       </c>
       <c r="S12" s="1">
-        <v>2.8983000000000002E-28</v>
-      </c>
-      <c r="T12" s="2">
-        <v>1</v>
+        <v>0.39529999999999998</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
       </c>
       <c r="U12" s="1">
-        <v>3.3134999999999998E-38</v>
-      </c>
-      <c r="V12" s="2">
-        <v>1</v>
+        <v>5.2400000000000002E-2</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
       </c>
       <c r="W12" s="1">
-        <v>2.9907999999999999E-5</v>
+        <v>0.78659999999999997</v>
       </c>
       <c r="X12" s="2">
         <v>1</v>
       </c>
       <c r="Y12" s="1">
-        <v>4.4576000000000002E-98</v>
+        <v>2.8E-3</v>
       </c>
       <c r="Z12">
         <v>0</v>

</xml_diff>